<commit_message>
Mass matrix and results
</commit_message>
<xml_diff>
--- a/Compiled standard test results/Composites/quantity recovery/thin quad/square_plate_sym_200x200.gid/square plate composite quantity recovery.xlsx
+++ b/Compiled standard test results/Composites/quantity recovery/thin quad/square_plate_sym_200x200.gid/square plate composite quantity recovery.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Desktop\TUM\Thesis\Development\Thin Quad\Composites\square_plate_sym_200x200.gid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Desktop\TUM\Thesis\Thesis\Compiled standard test results\Composites\quantity recovery\thin quad\square_plate_sym_200x200.gid\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1008,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B26:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q39" sqref="Q39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1184,7 +1184,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="L37">
-        <f>J37</f>
+        <f>C30/C28/F28</f>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="N37">

</xml_diff>